<commit_message>
added logreg and xgb submissions for center cv
</commit_message>
<xml_diff>
--- a/submissions/Overview_Submissions.xlsx
+++ b/submissions/Overview_Submissions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A74F185-DF0E-6D4C-9C0A-C1D1D29D818A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0852BF8B-486E-6B40-B318-185680082F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{2C151FD9-DA6B-A949-988F-18CD046A8920}"/>
+    <workbookView xWindow="1620" yWindow="760" windowWidth="28620" windowHeight="17300" xr2:uid="{2C151FD9-DA6B-A949-988F-18CD046A8920}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="49">
   <si>
     <t>File Name</t>
   </si>
@@ -150,6 +150,39 @@
   </si>
   <si>
     <t>Feb. 8, 2023, 9:01 a.m.</t>
+  </si>
+  <si>
+    <t>2023-02-16-2049_log_reg_centers.csv</t>
+  </si>
+  <si>
+    <t>2023-02-16-2136_xgb_centers.csv</t>
+  </si>
+  <si>
+    <t>2023-02-21-2055_xgb_centers_nohyp.csv</t>
+  </si>
+  <si>
+    <t>1 x 3</t>
+  </si>
+  <si>
+    <t>weakly supervision with cv centers</t>
+  </si>
+  <si>
+    <t>Feb. 16, 2023, 7:51 p.m.</t>
+  </si>
+  <si>
+    <t>Feb. 16, 2023, 8:37 p.m.</t>
+  </si>
+  <si>
+    <t>Feb. 21, 2023, 7:58 p.m.</t>
+  </si>
+  <si>
+    <t>0.601 (0.019)</t>
+  </si>
+  <si>
+    <t>0.597 (0.003)</t>
+  </si>
+  <si>
+    <t>0.608 (0.029)</t>
   </si>
 </sst>
 </file>
@@ -205,8 +238,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}" name="Tabelle1" displayName="Tabelle1" ref="A1:I8" totalsRowShown="0">
-  <autoFilter ref="A1:I8" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}" name="Tabelle1" displayName="Tabelle1" ref="A1:I11" totalsRowShown="0">
+  <autoFilter ref="A1:I11" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{38D19723-0BAA-CE43-BE05-765B83CC137A}" name="File Name"/>
     <tableColumn id="2" xr3:uid="{2BB12BDD-47FD-9E46-B0D7-3395F6FDCD6C}" name="Model"/>
@@ -519,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC84BD5-5F5D-1B48-A83A-0B338E19F0D5}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -766,6 +799,93 @@
         <v>15</v>
       </c>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9">
+        <v>0.63100000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10">
+        <v>0.58699999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" t="s">
+        <v>45</v>
+      </c>
+      <c r="I11">
+        <v>0.59899999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added submission for RF with average over tiles before prediction
</commit_message>
<xml_diff>
--- a/submissions/Overview_Submissions.xlsx
+++ b/submissions/Overview_Submissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F37EB88-9D68-E74C-895E-E60FF620F874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F019DA74-332E-FA48-9384-E89D85247B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="760" windowWidth="28620" windowHeight="17300" xr2:uid="{2C151FD9-DA6B-A949-988F-18CD046A8920}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
   <si>
     <t>File Name</t>
   </si>
@@ -195,6 +195,18 @@
   </si>
   <si>
     <t>0.611 (0.018)</t>
+  </si>
+  <si>
+    <t>weakly supervision with cv centers &amp; average before predictions</t>
+  </si>
+  <si>
+    <t>2023-02-27-1906_RF_centers_agg_pred.csv</t>
+  </si>
+  <si>
+    <t>0.609 (0.016)</t>
+  </si>
+  <si>
+    <t>Feb. 27, 2023, 6:20 p.m.</t>
   </si>
 </sst>
 </file>
@@ -250,8 +262,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}" name="Tabelle1" displayName="Tabelle1" ref="A1:I12" totalsRowShown="0">
-  <autoFilter ref="A1:I12" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}" name="Tabelle1" displayName="Tabelle1" ref="A1:I13" totalsRowShown="0">
+  <autoFilter ref="A1:I13" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{38D19723-0BAA-CE43-BE05-765B83CC137A}" name="File Name"/>
     <tableColumn id="2" xr3:uid="{2BB12BDD-47FD-9E46-B0D7-3395F6FDCD6C}" name="Model"/>
@@ -564,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC84BD5-5F5D-1B48-A83A-0B338E19F0D5}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -927,6 +939,35 @@
         <v>0.60099999999999998</v>
       </c>
     </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13">
+        <v>0.60499999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added RF submission with less features
</commit_message>
<xml_diff>
--- a/submissions/Overview_Submissions.xlsx
+++ b/submissions/Overview_Submissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F019DA74-332E-FA48-9384-E89D85247B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24ABC868-B68E-FF4A-8A93-E0A54546E55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="760" windowWidth="28620" windowHeight="17300" xr2:uid="{2C151FD9-DA6B-A949-988F-18CD046A8920}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
   <si>
     <t>File Name</t>
   </si>
@@ -207,6 +207,18 @@
   </si>
   <si>
     <t>Feb. 27, 2023, 6:20 p.m.</t>
+  </si>
+  <si>
+    <t>max_features="log2"</t>
+  </si>
+  <si>
+    <t>0.619 (0.022)</t>
+  </si>
+  <si>
+    <t>Feb. 28, 2023, 11:24 a.m.</t>
+  </si>
+  <si>
+    <t>2023-02-28-1210_RF_centers_less_feat.csv</t>
   </si>
 </sst>
 </file>
@@ -262,8 +274,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}" name="Tabelle1" displayName="Tabelle1" ref="A1:I13" totalsRowShown="0">
-  <autoFilter ref="A1:I13" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}" name="Tabelle1" displayName="Tabelle1" ref="A1:I14" totalsRowShown="0">
+  <autoFilter ref="A1:I14" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{38D19723-0BAA-CE43-BE05-765B83CC137A}" name="File Name"/>
     <tableColumn id="2" xr3:uid="{2BB12BDD-47FD-9E46-B0D7-3395F6FDCD6C}" name="Model"/>
@@ -576,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC84BD5-5F5D-1B48-A83A-0B338E19F0D5}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -968,6 +980,35 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14">
+        <v>0.59099999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
added RF submissions with class weights
</commit_message>
<xml_diff>
--- a/submissions/Overview_Submissions.xlsx
+++ b/submissions/Overview_Submissions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariastoelben/Documents/04_Studium/04_X-HEC Master 2022/M1/FS23/ENS Data Challenge/enschallenge2023/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24ABC868-B68E-FF4A-8A93-E0A54546E55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EBC7C6-52CB-A54B-8A90-600BFAC69544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1620" yWindow="760" windowWidth="28620" windowHeight="17300" xr2:uid="{2C151FD9-DA6B-A949-988F-18CD046A8920}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="69">
   <si>
     <t>File Name</t>
   </si>
@@ -219,6 +219,30 @@
   </si>
   <si>
     <t>2023-02-28-1210_RF_centers_less_feat.csv</t>
+  </si>
+  <si>
+    <t>2023-03-02-2013_RF_class_weights.csv</t>
+  </si>
+  <si>
+    <t>2023-03-02-2054_RF_class_weights.csv</t>
+  </si>
+  <si>
+    <t>0.620 (0.015)</t>
+  </si>
+  <si>
+    <t>0.622 (0.010)</t>
+  </si>
+  <si>
+    <t>max_features=1, n_jobs=6, class_weight={0:.35, 1:.65}</t>
+  </si>
+  <si>
+    <t>max_features=1, n_jobs=6, class_weight={0:.1, 1:.9}</t>
+  </si>
+  <si>
+    <t>March 2, 2023, 7:14 p.m.</t>
+  </si>
+  <si>
+    <t>March 2, 2023, 7:55 p.m.</t>
   </si>
 </sst>
 </file>
@@ -274,8 +298,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}" name="Tabelle1" displayName="Tabelle1" ref="A1:I14" totalsRowShown="0">
-  <autoFilter ref="A1:I14" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}" name="Tabelle1" displayName="Tabelle1" ref="A1:I16" totalsRowShown="0">
+  <autoFilter ref="A1:I16" xr:uid="{27C4B76E-8442-D34F-A1B0-0EC71A610050}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{38D19723-0BAA-CE43-BE05-765B83CC137A}" name="File Name"/>
     <tableColumn id="2" xr3:uid="{2BB12BDD-47FD-9E46-B0D7-3395F6FDCD6C}" name="Model"/>
@@ -588,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC84BD5-5F5D-1B48-A83A-0B338E19F0D5}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,6 +1033,64 @@
         <v>0.59099999999999997</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15">
+        <v>0.59799999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16">
+        <v>0.59399999999999997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>